<commit_message>
updated study 1 batch processing to include no cutoff frequency trials
</commit_message>
<xml_diff>
--- a/analyses/study_1/signal_conditioning_filter_cutoffs.xlsx
+++ b/analyses/study_1/signal_conditioning_filter_cutoffs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevenhirsch/Documents/force_plate_analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevenhirsch/Documents/force-plate-jump-analyses/analyses/study_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29908264-A5EE-DC4B-A0C5-3758A20205B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFB1A29-8E9A-5B4C-98A8-A9042E0966C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22900" yWindow="9500" windowWidth="29040" windowHeight="15840" xr2:uid="{029AE6D5-94AD-4E1D-8C68-365F27F4AF5A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20360" xr2:uid="{029AE6D5-94AD-4E1D-8C68-365F27F4AF5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="132">
   <si>
     <t>F01_CTRL1</t>
   </si>
@@ -426,6 +426,12 @@
   </si>
   <si>
     <t>literature_cutoff</t>
+  </si>
+  <si>
+    <t>no_cutoff</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -881,7 +887,7 @@
   <dimension ref="A1:BO16384"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -911,6 +917,9 @@
       <c r="E1" s="13" t="s">
         <v>129</v>
       </c>
+      <c r="F1" s="14" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="2" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -928,6 +937,9 @@
       <c r="E2" s="4">
         <v>50</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="3" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -945,6 +957,9 @@
       <c r="E3" s="4">
         <v>50</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="4" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -962,6 +977,9 @@
       <c r="E4" s="4">
         <v>50</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="BO4" s="2"/>
     </row>
     <row r="5" spans="1:67" x14ac:dyDescent="0.2">
@@ -980,6 +998,9 @@
       <c r="E5" s="4">
         <v>50</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="BO5" s="2"/>
     </row>
     <row r="6" spans="1:67" x14ac:dyDescent="0.2">
@@ -998,6 +1019,9 @@
       <c r="E6" s="4">
         <v>50</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="BN6" s="12"/>
       <c r="BO6" s="3"/>
     </row>
@@ -1017,6 +1041,9 @@
       <c r="E7" s="7">
         <v>50</v>
       </c>
+      <c r="F7" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="BN7" s="12"/>
       <c r="BO7" s="3"/>
     </row>
@@ -1036,6 +1063,9 @@
       <c r="E8" s="7">
         <v>50</v>
       </c>
+      <c r="F8" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="BN8" s="12"/>
       <c r="BO8" s="3"/>
     </row>
@@ -1055,6 +1085,9 @@
       <c r="E9" s="7">
         <v>50</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="10" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
@@ -1072,6 +1105,9 @@
       <c r="E10" s="7">
         <v>50</v>
       </c>
+      <c r="F10" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="11" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
@@ -1089,6 +1125,9 @@
       <c r="E11" s="7">
         <v>50</v>
       </c>
+      <c r="F11" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="12" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
@@ -1106,6 +1145,9 @@
       <c r="E12" s="4">
         <v>50</v>
       </c>
+      <c r="F12" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="13" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
@@ -1123,6 +1165,9 @@
       <c r="E13" s="4">
         <v>50</v>
       </c>
+      <c r="F13" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="14" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
@@ -1140,6 +1185,9 @@
       <c r="E14" s="4">
         <v>50</v>
       </c>
+      <c r="F14" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="15" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
@@ -1157,6 +1205,9 @@
       <c r="E15" s="4">
         <v>50</v>
       </c>
+      <c r="F15" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="16" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
@@ -1174,8 +1225,11 @@
       <c r="E16" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
@@ -1191,8 +1245,11 @@
       <c r="E17" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>16</v>
       </c>
@@ -1208,8 +1265,11 @@
       <c r="E18" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>17</v>
       </c>
@@ -1225,8 +1285,11 @@
       <c r="E19" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>18</v>
       </c>
@@ -1242,8 +1305,11 @@
       <c r="E20" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>20</v>
       </c>
@@ -1259,8 +1325,11 @@
       <c r="E21" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
@@ -1276,8 +1345,11 @@
       <c r="E22" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>22</v>
       </c>
@@ -1293,8 +1365,11 @@
       <c r="E23" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>23</v>
       </c>
@@ -1310,8 +1385,11 @@
       <c r="E24" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>24</v>
       </c>
@@ -1327,8 +1405,11 @@
       <c r="E25" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>19</v>
       </c>
@@ -1344,8 +1425,11 @@
       <c r="E26" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>25</v>
       </c>
@@ -1361,8 +1445,11 @@
       <c r="E27" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>26</v>
       </c>
@@ -1378,8 +1465,11 @@
       <c r="E28" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>27</v>
       </c>
@@ -1395,8 +1485,11 @@
       <c r="E29" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>28</v>
       </c>
@@ -1412,8 +1505,11 @@
       <c r="E30" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>29</v>
       </c>
@@ -1429,8 +1525,11 @@
       <c r="E31" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>30</v>
       </c>
@@ -1446,8 +1545,11 @@
       <c r="E32" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>31</v>
       </c>
@@ -1463,8 +1565,11 @@
       <c r="E33" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>32</v>
       </c>
@@ -1480,8 +1585,11 @@
       <c r="E34" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>33</v>
       </c>
@@ -1497,8 +1605,11 @@
       <c r="E35" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>34</v>
       </c>
@@ -1514,8 +1625,11 @@
       <c r="E36" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>35</v>
       </c>
@@ -1531,8 +1645,11 @@
       <c r="E37" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>36</v>
       </c>
@@ -1548,8 +1665,11 @@
       <c r="E38" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>37</v>
       </c>
@@ -1565,8 +1685,11 @@
       <c r="E39" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>38</v>
       </c>
@@ -1582,8 +1705,11 @@
       <c r="E40" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>39</v>
       </c>
@@ -1599,8 +1725,11 @@
       <c r="E41" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>40</v>
       </c>
@@ -1616,8 +1745,11 @@
       <c r="E42" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>41</v>
       </c>
@@ -1633,8 +1765,11 @@
       <c r="E43" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>42</v>
       </c>
@@ -1650,8 +1785,11 @@
       <c r="E44" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>43</v>
       </c>
@@ -1667,8 +1805,11 @@
       <c r="E45" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>44</v>
       </c>
@@ -1684,8 +1825,11 @@
       <c r="E46" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>45</v>
       </c>
@@ -1701,8 +1845,11 @@
       <c r="E47" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>46</v>
       </c>
@@ -1718,8 +1865,11 @@
       <c r="E48" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>47</v>
       </c>
@@ -1735,8 +1885,11 @@
       <c r="E49" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>48</v>
       </c>
@@ -1752,8 +1905,11 @@
       <c r="E50" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>49</v>
       </c>
@@ -1769,8 +1925,11 @@
       <c r="E51" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>50</v>
       </c>
@@ -1786,8 +1945,11 @@
       <c r="E52" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>51</v>
       </c>
@@ -1803,8 +1965,11 @@
       <c r="E53" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>52</v>
       </c>
@@ -1820,8 +1985,11 @@
       <c r="E54" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>53</v>
       </c>
@@ -1837,8 +2005,11 @@
       <c r="E55" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>54</v>
       </c>
@@ -1854,8 +2025,11 @@
       <c r="E56" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>55</v>
       </c>
@@ -1871,8 +2045,11 @@
       <c r="E57" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>56</v>
       </c>
@@ -1888,8 +2065,11 @@
       <c r="E58" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>57</v>
       </c>
@@ -1905,8 +2085,11 @@
       <c r="E59" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
         <v>58</v>
       </c>
@@ -1922,8 +2105,11 @@
       <c r="E60" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
         <v>59</v>
       </c>
@@ -1939,8 +2125,11 @@
       <c r="E61" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>60</v>
       </c>
@@ -1956,8 +2145,11 @@
       <c r="E62" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>61</v>
       </c>
@@ -1973,8 +2165,11 @@
       <c r="E63" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>62</v>
       </c>
@@ -1990,8 +2185,11 @@
       <c r="E64" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>63</v>
       </c>
@@ -2007,8 +2205,11 @@
       <c r="E65" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>64</v>
       </c>
@@ -2024,8 +2225,11 @@
       <c r="E66" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
         <v>65</v>
       </c>
@@ -2041,8 +2245,11 @@
       <c r="E67" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
         <v>66</v>
       </c>
@@ -2058,8 +2265,11 @@
       <c r="E68" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
         <v>67</v>
       </c>
@@ -2075,8 +2285,11 @@
       <c r="E69" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
         <v>68</v>
       </c>
@@ -2092,8 +2305,11 @@
       <c r="E70" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
         <v>69</v>
       </c>
@@ -2109,8 +2325,11 @@
       <c r="E71" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>70</v>
       </c>
@@ -2126,8 +2345,11 @@
       <c r="E72" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>71</v>
       </c>
@@ -2143,8 +2365,11 @@
       <c r="E73" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>72</v>
       </c>
@@ -2160,8 +2385,11 @@
       <c r="E74" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>73</v>
       </c>
@@ -2177,8 +2405,11 @@
       <c r="E75" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>74</v>
       </c>
@@ -2194,8 +2425,11 @@
       <c r="E76" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
         <v>75</v>
       </c>
@@ -2211,8 +2445,11 @@
       <c r="E77" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
         <v>76</v>
       </c>
@@ -2228,8 +2465,11 @@
       <c r="E78" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
         <v>77</v>
       </c>
@@ -2245,8 +2485,11 @@
       <c r="E79" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
         <v>78</v>
       </c>
@@ -2262,8 +2505,11 @@
       <c r="E80" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
         <v>79</v>
       </c>
@@ -2279,8 +2525,11 @@
       <c r="E81" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>80</v>
       </c>
@@ -2296,8 +2545,11 @@
       <c r="E82" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>81</v>
       </c>
@@ -2313,8 +2565,11 @@
       <c r="E83" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>82</v>
       </c>
@@ -2330,8 +2585,11 @@
       <c r="E84" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>83</v>
       </c>
@@ -2347,8 +2605,11 @@
       <c r="E85" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>84</v>
       </c>
@@ -2364,8 +2625,11 @@
       <c r="E86" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F86" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
         <v>85</v>
       </c>
@@ -2381,8 +2645,11 @@
       <c r="E87" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F87" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
         <v>86</v>
       </c>
@@ -2398,8 +2665,11 @@
       <c r="E88" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F88" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
         <v>87</v>
       </c>
@@ -2415,8 +2685,11 @@
       <c r="E89" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F89" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
         <v>88</v>
       </c>
@@ -2432,8 +2705,11 @@
       <c r="E90" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F90" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
         <v>89</v>
       </c>
@@ -2449,8 +2725,11 @@
       <c r="E91" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F91" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>90</v>
       </c>
@@ -2466,8 +2745,11 @@
       <c r="E92" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F92" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>91</v>
       </c>
@@ -2483,8 +2765,11 @@
       <c r="E93" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F93" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>92</v>
       </c>
@@ -2500,8 +2785,11 @@
       <c r="E94" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F94" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>93</v>
       </c>
@@ -2517,8 +2805,11 @@
       <c r="E95" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F95" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>94</v>
       </c>
@@ -2534,8 +2825,11 @@
       <c r="E96" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F96" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
         <v>95</v>
       </c>
@@ -2551,8 +2845,11 @@
       <c r="E97" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F97" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
         <v>96</v>
       </c>
@@ -2568,8 +2865,11 @@
       <c r="E98" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F98" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
         <v>97</v>
       </c>
@@ -2585,8 +2885,11 @@
       <c r="E99" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F99" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
         <v>98</v>
       </c>
@@ -2602,8 +2905,11 @@
       <c r="E100" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F100" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
         <v>99</v>
       </c>
@@ -2619,8 +2925,11 @@
       <c r="E101" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F101" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>100</v>
       </c>
@@ -2636,8 +2945,11 @@
       <c r="E102" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F102" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>101</v>
       </c>
@@ -2653,8 +2965,11 @@
       <c r="E103" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F103" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>102</v>
       </c>
@@ -2670,8 +2985,11 @@
       <c r="E104" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F104" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>103</v>
       </c>
@@ -2687,8 +3005,11 @@
       <c r="E105" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F105" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>104</v>
       </c>
@@ -2704,8 +3025,11 @@
       <c r="E106" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F106" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="7" t="s">
         <v>105</v>
       </c>
@@ -2721,8 +3045,11 @@
       <c r="E107" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F107" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="7" t="s">
         <v>106</v>
       </c>
@@ -2738,8 +3065,11 @@
       <c r="E108" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F108" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="7" t="s">
         <v>107</v>
       </c>
@@ -2755,8 +3085,11 @@
       <c r="E109" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F109" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
         <v>108</v>
       </c>
@@ -2772,8 +3105,11 @@
       <c r="E110" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F110" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
         <v>109</v>
       </c>
@@ -2789,8 +3125,11 @@
       <c r="E111" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F111" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>110</v>
       </c>
@@ -2806,8 +3145,11 @@
       <c r="E112" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F112" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>111</v>
       </c>
@@ -2823,8 +3165,11 @@
       <c r="E113" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F113" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>112</v>
       </c>
@@ -2840,8 +3185,11 @@
       <c r="E114" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F114" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>113</v>
       </c>
@@ -2857,8 +3205,11 @@
       <c r="E115" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F115" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>114</v>
       </c>
@@ -2874,8 +3225,11 @@
       <c r="E116" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F116" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="7" t="s">
         <v>115</v>
       </c>
@@ -2891,8 +3245,11 @@
       <c r="E117" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F117" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="7" t="s">
         <v>116</v>
       </c>
@@ -2908,8 +3265,11 @@
       <c r="E118" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F118" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="7" t="s">
         <v>117</v>
       </c>
@@ -2925,8 +3285,11 @@
       <c r="E119" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F119" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
         <v>118</v>
       </c>
@@ -2942,8 +3305,11 @@
       <c r="E120" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F120" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="7" t="s">
         <v>119</v>
       </c>
@@ -2959,8 +3325,11 @@
       <c r="E121" s="7">
         <v>50</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F121" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
         <v>120</v>
       </c>
@@ -2976,8 +3345,11 @@
       <c r="E122" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F122" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>121</v>
       </c>
@@ -2993,8 +3365,11 @@
       <c r="E123" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F123" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>122</v>
       </c>
@@ -3010,8 +3385,11 @@
       <c r="E124" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F124" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
         <v>123</v>
       </c>
@@ -3027,8 +3405,11 @@
       <c r="E125" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F125" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
         <v>124</v>
       </c>
@@ -3044,11 +3425,14 @@
       <c r="E126" s="4">
         <v>50</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F126" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>